<commit_message>
Stats for all XLSXes, loss charts for 50/1-25
</commit_message>
<xml_diff>
--- a/experiment_results/trajectory_2021-06-07T13:40:45.585921.xlsx
+++ b/experiment_results/trajectory_2021-06-07T13:40:45.585921.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
   <si>
     <t xml:space="preserve">50 epochs, depths 25-50</t>
   </si>
@@ -633,6 +633,18 @@
   <si>
     <t xml:space="preserve">&lt;Genome {'input_shape': (3, 32, 32), 'output_feature_depth': 10, 'genes': [&lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(3, 32, 32)], '_DepSepConvNode__input_shape': (3, 32, 32), '_DepSepConvNode__output_feature_depth': 256, 'kernel_size': 3}&gt;, 'input_indices': [-1], 'input_shapes': [(3, 32, 32)]}&gt;, &lt;Gene {'node': &lt;CatNode {'input_shapes': [(3, 32, 32), (3, 32, 32)]}&gt;, 'input_indices': [-1, -1], 'input_shapes': [(3, 32, 32), (3, 32, 32)]}&gt;, &lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(6, 3, 3)], '_DepSepConvNode__input_shape': (6, 3, 3), '_DepSepConvNode__output_feature_depth': 128, 'kernel_size': 3}&gt;, 'input_indices': [1], 'input_shapes': [(6, 3, 3)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(3, 32, 32), (128, 3, 3)]}&gt;, 'input_indices': [-1, 2], 'input_shapes': [(3, 32, 32), (128, 3, 3)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(6, 3, 3), (3, 32, 32)]}&gt;, 'input_indices': [1, -1], 'input_shapes': [(6, 3, 3), (3, 32, 32)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(6, 6, 6), (6, 3, 3)]}&gt;, 'input_indices': [4, 1], 'input_shapes': [(6, 6, 6), (6, 3, 3)]}&gt;, &lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(3, 32, 32)], '_DepSepConvNode__input_shape': (3, 32, 32), '_DepSepConvNode__output_feature_depth': 32, 'kernel_size': 3}&gt;, 'input_indices': [-1], 'input_shapes': [(3, 32, 32)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(128, 3, 3)]}&gt;, 'input_indices': [2], 'input_shapes': [(128, 3, 3)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(256, 32, 32)]}&gt;, 'input_indices': [0], 'input_shapes': [(256, 32, 32)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(128, 128, 128), (128, 1, 1)]}&gt;, 'input_indices': [3, 7], 'input_shapes': [(128, 128, 128), (128, 1, 1)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(256, 32, 32)]}&gt;, 'input_indices': [0], 'input_shapes': [(256, 32, 32)]}&gt;, &lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(128, 3, 3)], '_DepSepConvNode__input_shape': (128, 3, 3), '_DepSepConvNode__output_feature_depth': 64, 'kernel_size': 3}&gt;, 'input_indices': [2], 'input_shapes': [(128, 3, 3)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(6, 6, 6), (128, 1, 1)]}&gt;, 'input_indices': [4, 7], 'input_shapes': [(6, 6, 6), (128, 1, 1)]}&gt;, &lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(6, 6, 6)], '_DepSepConvNode__input_shape': (6, 6, 6), '_DepSepConvNode__output_feature_depth': 64, 'kernel_size': 3}&gt;, 'input_indices': [4], 'input_shapes': [(6, 6, 6)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(3, 32, 32)]}&gt;, 'input_indices': [-1], 'input_shapes': [(3, 32, 32)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(64, 6, 6)]}&gt;, 'input_indices': [13], 'input_shapes': [(64, 6, 6)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(32, 32, 32)]}&gt;, 'input_indices': [6], 'input_shapes': [(32, 32, 32)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(32, 16, 16)]}&gt;, 'input_indices': [16], 'input_shapes': [(32, 16, 16)]}&gt;, &lt;Gene {'node': &lt;CatNode {'input_shapes': [(128, 1, 1), (256, 16, 16)]}&gt;, 'input_indices': [7, 8], 'input_shapes': [(128, 1, 1), (256, 16, 16)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(256, 32, 32)]}&gt;, 'input_indices': [0], 'input_shapes': [(256, 32, 32)]}&gt;, &lt;Gene {'node': &lt;CatNode {'input_shapes': [(6, 6, 6), (128, 128, 128)]}&gt;, 'input_indices': [5, 9], 'input_shapes': [(6, 6, 6), (128, 128, 128)]}&gt;, &lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(64, 3, 3)], '_DepSepConvNode__input_shape': (64, 3, 3), '_DepSepConvNode__output_feature_depth': 128, 'kernel_size': 5}&gt;, 'input_indices': [11], 'input_shapes': [(64, 3, 3)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(384, 256, 256)]}&gt;, 'input_indices': [18], 'input_shapes': [(384, 256, 256)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(32, 32, 32)]}&gt;, 'input_indices': [6], 'input_shapes': [(32, 32, 32)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(64, 6, 6)]}&gt;, 'input_indices': [13], 'input_shapes': [(64, 6, 6)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(32, 32, 32), (32, 16, 16)]}&gt;, 'input_indices': [6, 23], 'input_shapes': [(32, 32, 32), (32, 16, 16)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(128, 128, 128), (256, 16, 16)]}&gt;, 'input_indices': [3, 8], 'input_shapes': [(128, 128, 128), (256, 16, 16)]}&gt;, &lt;Gene {'node': &lt;ConvNode {'input_shapes': [(128, 128, 128)], '_ConvNode__input_shape': (128, 128, 128), '_ConvNode__output_feature_depth': 256, 'kernel_size': 3}&gt;, 'input_indices': [3], 'input_shapes': [(128, 128, 128)]}&gt;, &lt;Gene {'node': &lt;ConvNode {'input_shapes': [(256, 16, 16)], '_ConvNode__input_shape': (256, 16, 16), '_ConvNode__output_feature_depth': 32, 'kernel_size': 1}&gt;, 'input_indices': [19], 'input_shapes': [(256, 16, 16)]}&gt;, &lt;Gene {'node': &lt;SumNode {'input_shapes': [(128, 128, 128), (256, 16, 16)]}&gt;, 'input_indices': [12, 10], 'input_shapes': [(128, 128, 128), (256, 16, 16)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(64, 3, 3)]}&gt;, 'input_indices': [24], 'input_shapes': [(64, 3, 3)]}&gt;, &lt;Gene {'node': &lt;ConvNode {'input_shapes': [(3, 16, 16)], '_ConvNode__input_shape': (3, 16, 16), '_ConvNode__output_feature_depth': 128, 'kernel_size': 1}&gt;, 'input_indices': [14], 'input_shapes': [(3, 16, 16)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(128, 1, 1)]}&gt;, 'input_indices': [7], 'input_shapes': [(128, 1, 1)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(128, 1, 1)]}&gt;, 'input_indices': [32], 'input_shapes': [(128, 1, 1)]}&gt;, &lt;Gene {'node': &lt;ConvNode {'input_shapes': [(128, 1, 1)], '_ConvNode__input_shape': (128, 1, 1), '_ConvNode__output_feature_depth': 256, 'kernel_size': 3}&gt;, 'input_indices': [32], 'input_shapes': [(128, 1, 1)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(134, 128, 128)]}&gt;, 'input_indices': [20], 'input_shapes': [(134, 128, 128)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(256, 256, 256)]}&gt;, 'input_indices': [26], 'input_shapes': [(256, 256, 256)]}&gt;, &lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(128, 1, 1)], '_DepSepConvNode__input_shape': (128, 1, 1), '_DepSepConvNode__output_feature_depth': 128, 'kernel_size': 3}&gt;, 'input_indices': [32], 'input_shapes': [(128, 1, 1)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(134, 128, 128)]}&gt;, 'input_indices': [20], 'input_shapes': [(134, 128, 128)]}&gt;, &lt;Gene {'node': &lt;MaxPoolNode {'input_shapes': [(128, 3, 3)]}&gt;, 'input_indices': [2], 'input_shapes': [(128, 3, 3)]}&gt;, &lt;Gene {'node': &lt;DepSepConvNode {'input_shapes': [(64, 3, 3)], '_DepSepConvNode__input_shape': (64, 3, 3), '_DepSepConvNode__output_feature_depth': 128, 'kernel_size': 5}&gt;, 'input_indices': [11], 'input_shapes': [(64, 3, 3)]}&gt;, &lt;Gene {'node': &lt;AvgPoolNode {'input_shapes': [(3, 16, 16)]}&gt;, 'input_indices': [14], 'input_shapes': [(3, 16, 16)]}&gt;]}&gt;</t>
   </si>
+  <si>
+    <t xml:space="preserve">Average loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation to e100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation to v100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en/vn correlation</t>
+  </si>
 </sst>
 </file>
 
@@ -727,10 +739,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CY102"/>
+  <dimension ref="A1:CY109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BV63" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="GU104" activeCellId="0" sqref="CZ104:GU107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32162,6 +32174,1454 @@
         <v>1.40548384189606</v>
       </c>
     </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <f aca="false">AVERAGE(B4:B102)</f>
+        <v>9.98036691395923</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <f aca="false">AVERAGE(C4:C102)</f>
+        <v>1.8195481336478</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <f aca="false">AVERAGE(D4:D102)</f>
+        <v>1.70791911235963</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <f aca="false">AVERAGE(E4:E102)</f>
+        <v>1.63353581259949</v>
+      </c>
+      <c r="F104" s="0" t="n">
+        <f aca="false">AVERAGE(F4:F102)</f>
+        <v>1.57477293110857</v>
+      </c>
+      <c r="G104" s="0" t="n">
+        <f aca="false">AVERAGE(G4:G102)</f>
+        <v>1.52525532366049</v>
+      </c>
+      <c r="H104" s="0" t="n">
+        <f aca="false">AVERAGE(H4:H102)</f>
+        <v>1.48260707325406</v>
+      </c>
+      <c r="I104" s="0" t="n">
+        <f aca="false">AVERAGE(I4:I102)</f>
+        <v>1.44464159072048</v>
+      </c>
+      <c r="J104" s="0" t="n">
+        <f aca="false">AVERAGE(J4:J102)</f>
+        <v>1.40966962202631</v>
+      </c>
+      <c r="K104" s="0" t="n">
+        <f aca="false">AVERAGE(K4:K102)</f>
+        <v>1.37672697594672</v>
+      </c>
+      <c r="L104" s="0" t="n">
+        <f aca="false">AVERAGE(L4:L102)</f>
+        <v>1.34574320701638</v>
+      </c>
+      <c r="M104" s="0" t="n">
+        <f aca="false">AVERAGE(M4:M102)</f>
+        <v>1.31670308414132</v>
+      </c>
+      <c r="N104" s="0" t="n">
+        <f aca="false">AVERAGE(N4:N102)</f>
+        <v>1.28861234946684</v>
+      </c>
+      <c r="O104" s="0" t="n">
+        <f aca="false">AVERAGE(O4:O102)</f>
+        <v>1.2623649579708</v>
+      </c>
+      <c r="P104" s="0" t="n">
+        <f aca="false">AVERAGE(P4:P102)</f>
+        <v>1.23760359576254</v>
+      </c>
+      <c r="Q104" s="0" t="n">
+        <f aca="false">AVERAGE(Q4:Q102)</f>
+        <v>1.2114517372666</v>
+      </c>
+      <c r="R104" s="0" t="n">
+        <f aca="false">AVERAGE(R4:R102)</f>
+        <v>1.18654356144293</v>
+      </c>
+      <c r="S104" s="0" t="n">
+        <f aca="false">AVERAGE(S4:S102)</f>
+        <v>1.16359837970348</v>
+      </c>
+      <c r="T104" s="0" t="n">
+        <f aca="false">AVERAGE(T4:T102)</f>
+        <v>1.14069852624277</v>
+      </c>
+      <c r="U104" s="0" t="n">
+        <f aca="false">AVERAGE(U4:U102)</f>
+        <v>1.11914809661532</v>
+      </c>
+      <c r="V104" s="0" t="n">
+        <f aca="false">AVERAGE(V4:V102)</f>
+        <v>1.09732104645986</v>
+      </c>
+      <c r="W104" s="0" t="n">
+        <f aca="false">AVERAGE(W4:W102)</f>
+        <v>1.07621292673014</v>
+      </c>
+      <c r="X104" s="0" t="n">
+        <f aca="false">AVERAGE(X4:X102)</f>
+        <v>1.05448098825949</v>
+      </c>
+      <c r="Y104" s="0" t="n">
+        <f aca="false">AVERAGE(Y4:Y102)</f>
+        <v>1.0342009206246</v>
+      </c>
+      <c r="Z104" s="0" t="n">
+        <f aca="false">AVERAGE(Z4:Z102)</f>
+        <v>1.01523277960774</v>
+      </c>
+      <c r="AA104" s="0" t="n">
+        <f aca="false">AVERAGE(AA4:AA102)</f>
+        <v>0.997297193690419</v>
+      </c>
+      <c r="AB104" s="0" t="n">
+        <f aca="false">AVERAGE(AB4:AB102)</f>
+        <v>0.979901418047534</v>
+      </c>
+      <c r="AC104" s="0" t="n">
+        <f aca="false">AVERAGE(AC4:AC102)</f>
+        <v>0.961254642455547</v>
+      </c>
+      <c r="AD104" s="0" t="n">
+        <f aca="false">AVERAGE(AD4:AD102)</f>
+        <v>0.942773425130813</v>
+      </c>
+      <c r="AE104" s="0" t="n">
+        <f aca="false">AVERAGE(AE4:AE102)</f>
+        <v>0.923354492054763</v>
+      </c>
+      <c r="AF104" s="0" t="n">
+        <f aca="false">AVERAGE(AF4:AF102)</f>
+        <v>0.904046824787546</v>
+      </c>
+      <c r="AG104" s="0" t="n">
+        <f aca="false">AVERAGE(AG4:AG102)</f>
+        <v>0.88761805987804</v>
+      </c>
+      <c r="AH104" s="0" t="n">
+        <f aca="false">AVERAGE(AH4:AH102)</f>
+        <v>0.872662311389271</v>
+      </c>
+      <c r="AI104" s="0" t="n">
+        <f aca="false">AVERAGE(AI4:AI102)</f>
+        <v>0.858096556153591</v>
+      </c>
+      <c r="AJ104" s="0" t="n">
+        <f aca="false">AVERAGE(AJ4:AJ102)</f>
+        <v>0.844759767773947</v>
+      </c>
+      <c r="AK104" s="0" t="n">
+        <f aca="false">AVERAGE(AK4:AK102)</f>
+        <v>0.829520930592535</v>
+      </c>
+      <c r="AL104" s="0" t="n">
+        <f aca="false">AVERAGE(AL4:AL102)</f>
+        <v>0.812983873006276</v>
+      </c>
+      <c r="AM104" s="0" t="n">
+        <f aca="false">AVERAGE(AM4:AM102)</f>
+        <v>0.794515819400502</v>
+      </c>
+      <c r="AN104" s="0" t="n">
+        <f aca="false">AVERAGE(AN4:AN102)</f>
+        <v>0.780936468727746</v>
+      </c>
+      <c r="AO104" s="0" t="n">
+        <f aca="false">AVERAGE(AO4:AO102)</f>
+        <v>0.768088878770923</v>
+      </c>
+      <c r="AP104" s="0" t="n">
+        <f aca="false">AVERAGE(AP4:AP102)</f>
+        <v>0.754069332775396</v>
+      </c>
+      <c r="AQ104" s="0" t="n">
+        <f aca="false">AVERAGE(AQ4:AQ102)</f>
+        <v>0.740248033992071</v>
+      </c>
+      <c r="AR104" s="0" t="n">
+        <f aca="false">AVERAGE(AR4:AR102)</f>
+        <v>0.729012378416203</v>
+      </c>
+      <c r="AS104" s="0" t="n">
+        <f aca="false">AVERAGE(AS4:AS102)</f>
+        <v>0.715477631643128</v>
+      </c>
+      <c r="AT104" s="0" t="n">
+        <f aca="false">AVERAGE(AT4:AT102)</f>
+        <v>0.703439872290332</v>
+      </c>
+      <c r="AU104" s="0" t="n">
+        <f aca="false">AVERAGE(AU4:AU102)</f>
+        <v>0.692845224098872</v>
+      </c>
+      <c r="AV104" s="0" t="n">
+        <f aca="false">AVERAGE(AV4:AV102)</f>
+        <v>0.679917006957994</v>
+      </c>
+      <c r="AW104" s="0" t="n">
+        <f aca="false">AVERAGE(AW4:AW102)</f>
+        <v>0.670907037833593</v>
+      </c>
+      <c r="AX104" s="0" t="n">
+        <f aca="false">AVERAGE(AX4:AX102)</f>
+        <v>0.661905982762086</v>
+      </c>
+      <c r="AY104" s="0" t="n">
+        <f aca="false">AVERAGE(AY4:AY102)</f>
+        <v>0.649442725759023</v>
+      </c>
+      <c r="AZ104" s="0" t="n">
+        <f aca="false">AVERAGE(AZ4:AZ102)</f>
+        <v>0.638120162549471</v>
+      </c>
+      <c r="BA104" s="0" t="n">
+        <f aca="false">AVERAGE(BA4:BA102)</f>
+        <v>9.77877804004785</v>
+      </c>
+      <c r="BB104" s="0" t="n">
+        <f aca="false">AVERAGE(BB4:BB102)</f>
+        <v>1.81420030617955</v>
+      </c>
+      <c r="BC104" s="0" t="n">
+        <f aca="false">AVERAGE(BC4:BC102)</f>
+        <v>1.71623926812952</v>
+      </c>
+      <c r="BD104" s="0" t="n">
+        <f aca="false">AVERAGE(BD4:BD102)</f>
+        <v>1.65513713793321</v>
+      </c>
+      <c r="BE104" s="0" t="n">
+        <f aca="false">AVERAGE(BE4:BE102)</f>
+        <v>1.60931638876597</v>
+      </c>
+      <c r="BF104" s="0" t="n">
+        <f aca="false">AVERAGE(BF4:BF102)</f>
+        <v>1.57295204172231</v>
+      </c>
+      <c r="BG104" s="0" t="n">
+        <f aca="false">AVERAGE(BG4:BG102)</f>
+        <v>1.54308348111432</v>
+      </c>
+      <c r="BH104" s="0" t="n">
+        <f aca="false">AVERAGE(BH4:BH102)</f>
+        <v>1.51794986411779</v>
+      </c>
+      <c r="BI104" s="0" t="n">
+        <f aca="false">AVERAGE(BI4:BI102)</f>
+        <v>1.49619567273843</v>
+      </c>
+      <c r="BJ104" s="0" t="n">
+        <f aca="false">AVERAGE(BJ4:BJ102)</f>
+        <v>1.47699082499803</v>
+      </c>
+      <c r="BK104" s="0" t="n">
+        <f aca="false">AVERAGE(BK4:BK102)</f>
+        <v>1.46058357604826</v>
+      </c>
+      <c r="BL104" s="0" t="n">
+        <f aca="false">AVERAGE(BL4:BL102)</f>
+        <v>1.44687619233372</v>
+      </c>
+      <c r="BM104" s="0" t="n">
+        <f aca="false">AVERAGE(BM4:BM102)</f>
+        <v>1.43461169979789</v>
+      </c>
+      <c r="BN104" s="0" t="n">
+        <f aca="false">AVERAGE(BN4:BN102)</f>
+        <v>1.42411313996171</v>
+      </c>
+      <c r="BO104" s="0" t="n">
+        <f aca="false">AVERAGE(BO4:BO102)</f>
+        <v>1.41612789606807</v>
+      </c>
+      <c r="BP104" s="0" t="n">
+        <f aca="false">AVERAGE(BP4:BP102)</f>
+        <v>1.40719639291667</v>
+      </c>
+      <c r="BQ104" s="0" t="n">
+        <f aca="false">AVERAGE(BQ4:BQ102)</f>
+        <v>1.3993765645557</v>
+      </c>
+      <c r="BR104" s="0" t="n">
+        <f aca="false">AVERAGE(BR4:BR102)</f>
+        <v>1.39320217720186</v>
+      </c>
+      <c r="BS104" s="0" t="n">
+        <f aca="false">AVERAGE(BS4:BS102)</f>
+        <v>1.38794830953232</v>
+      </c>
+      <c r="BT104" s="0" t="n">
+        <f aca="false">AVERAGE(BT4:BT102)</f>
+        <v>1.38561854217992</v>
+      </c>
+      <c r="BU104" s="0" t="n">
+        <f aca="false">AVERAGE(BU4:BU102)</f>
+        <v>1.38086958605834</v>
+      </c>
+      <c r="BV104" s="0" t="n">
+        <f aca="false">AVERAGE(BV4:BV102)</f>
+        <v>1.37909238266222</v>
+      </c>
+      <c r="BW104" s="0" t="n">
+        <f aca="false">AVERAGE(BW4:BW102)</f>
+        <v>1.37604503318517</v>
+      </c>
+      <c r="BX104" s="0" t="n">
+        <f aca="false">AVERAGE(BX4:BX102)</f>
+        <v>1.3739386399587</v>
+      </c>
+      <c r="BY104" s="0" t="n">
+        <f aca="false">AVERAGE(BY4:BY102)</f>
+        <v>1.37384675849568</v>
+      </c>
+      <c r="BZ104" s="0" t="n">
+        <f aca="false">AVERAGE(BZ4:BZ102)</f>
+        <v>1.37601635191176</v>
+      </c>
+      <c r="CA104" s="0" t="n">
+        <f aca="false">AVERAGE(CA4:CA102)</f>
+        <v>1.37758892593962</v>
+      </c>
+      <c r="CB104" s="0" t="n">
+        <f aca="false">AVERAGE(CB4:CB102)</f>
+        <v>1.37943553924561</v>
+      </c>
+      <c r="CC104" s="0" t="n">
+        <f aca="false">AVERAGE(CC4:CC102)</f>
+        <v>1.38266552819146</v>
+      </c>
+      <c r="CD104" s="0" t="n">
+        <f aca="false">AVERAGE(CD4:CD102)</f>
+        <v>1.38330049105365</v>
+      </c>
+      <c r="CE104" s="0" t="n">
+        <f aca="false">AVERAGE(CE4:CE102)</f>
+        <v>1.38364231466043</v>
+      </c>
+      <c r="CF104" s="0" t="n">
+        <f aca="false">AVERAGE(CF4:CF102)</f>
+        <v>1.38743354575803</v>
+      </c>
+      <c r="CG104" s="0" t="n">
+        <f aca="false">AVERAGE(CG4:CG102)</f>
+        <v>1.39547783798642</v>
+      </c>
+      <c r="CH104" s="0" t="n">
+        <f aca="false">AVERAGE(CH4:CH102)</f>
+        <v>1.40182473201944</v>
+      </c>
+      <c r="CI104" s="0" t="n">
+        <f aca="false">AVERAGE(CI4:CI102)</f>
+        <v>1.40767014508296</v>
+      </c>
+      <c r="CJ104" s="0" t="n">
+        <f aca="false">AVERAGE(CJ4:CJ102)</f>
+        <v>1.41232181799532</v>
+      </c>
+      <c r="CK104" s="0" t="n">
+        <f aca="false">AVERAGE(CK4:CK102)</f>
+        <v>1.41478043975252</v>
+      </c>
+      <c r="CL104" s="0" t="n">
+        <f aca="false">AVERAGE(CL4:CL102)</f>
+        <v>1.41464555865586</v>
+      </c>
+      <c r="CM104" s="0" t="n">
+        <f aca="false">AVERAGE(CM4:CM102)</f>
+        <v>1.41960767423264</v>
+      </c>
+      <c r="CN104" s="0" t="n">
+        <f aca="false">AVERAGE(CN4:CN102)</f>
+        <v>1.42771290769481</v>
+      </c>
+      <c r="CO104" s="0" t="n">
+        <f aca="false">AVERAGE(CO4:CO102)</f>
+        <v>1.43145209972305</v>
+      </c>
+      <c r="CP104" s="0" t="n">
+        <f aca="false">AVERAGE(CP4:CP102)</f>
+        <v>1.43727097125969</v>
+      </c>
+      <c r="CQ104" s="0" t="n">
+        <f aca="false">AVERAGE(CQ4:CQ102)</f>
+        <v>1.44815308638293</v>
+      </c>
+      <c r="CR104" s="0" t="n">
+        <f aca="false">AVERAGE(CR4:CR102)</f>
+        <v>1.45337516852099</v>
+      </c>
+      <c r="CS104" s="0" t="n">
+        <f aca="false">AVERAGE(CS4:CS102)</f>
+        <v>1.46138071411788</v>
+      </c>
+      <c r="CT104" s="0" t="n">
+        <f aca="false">AVERAGE(CT4:CT102)</f>
+        <v>1.4688615473834</v>
+      </c>
+      <c r="CU104" s="0" t="n">
+        <f aca="false">AVERAGE(CU4:CU102)</f>
+        <v>1.4722147337114</v>
+      </c>
+      <c r="CV104" s="0" t="n">
+        <f aca="false">AVERAGE(CV4:CV102)</f>
+        <v>1.48149735759003</v>
+      </c>
+      <c r="CW104" s="0" t="n">
+        <f aca="false">AVERAGE(CW4:CW102)</f>
+        <v>1.48949580601972</v>
+      </c>
+      <c r="CX104" s="0" t="n">
+        <f aca="false">AVERAGE(CX4:CX102)</f>
+        <v>1.49327897543859</v>
+      </c>
+      <c r="CY104" s="0" t="n">
+        <f aca="false">AVERAGE(CY4:CY102)</f>
+        <v>1.49771352970239</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <f aca="false">CORREL(B4:B102,$AZ4:$AZ102)</f>
+        <v>-0.229402906142131</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <f aca="false">CORREL(C4:C102,$AZ4:$AZ102)</f>
+        <v>0.816397644711634</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <f aca="false">CORREL(D4:D102,$AZ4:$AZ102)</f>
+        <v>0.827283035248216</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <f aca="false">CORREL(E4:E102,$AZ4:$AZ102)</f>
+        <v>0.846300913861774</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <f aca="false">CORREL(F4:F102,$AZ4:$AZ102)</f>
+        <v>0.865444143326582</v>
+      </c>
+      <c r="G106" s="0" t="n">
+        <f aca="false">CORREL(G4:G102,$AZ4:$AZ102)</f>
+        <v>0.880156790397174</v>
+      </c>
+      <c r="H106" s="0" t="n">
+        <f aca="false">CORREL(H4:H102,$AZ4:$AZ102)</f>
+        <v>0.891439453087092</v>
+      </c>
+      <c r="I106" s="0" t="n">
+        <f aca="false">CORREL(I4:I102,$AZ4:$AZ102)</f>
+        <v>0.897980646723052</v>
+      </c>
+      <c r="J106" s="0" t="n">
+        <f aca="false">CORREL(J4:J102,$AZ4:$AZ102)</f>
+        <v>0.903451004761236</v>
+      </c>
+      <c r="K106" s="0" t="n">
+        <f aca="false">CORREL(K4:K102,$AZ4:$AZ102)</f>
+        <v>0.906210314719782</v>
+      </c>
+      <c r="L106" s="0" t="n">
+        <f aca="false">CORREL(L4:L102,$AZ4:$AZ102)</f>
+        <v>0.907596632102183</v>
+      </c>
+      <c r="M106" s="0" t="n">
+        <f aca="false">CORREL(M4:M102,$AZ4:$AZ102)</f>
+        <v>0.907703679269821</v>
+      </c>
+      <c r="N106" s="0" t="n">
+        <f aca="false">CORREL(N4:N102,$AZ4:$AZ102)</f>
+        <v>0.90752572954133</v>
+      </c>
+      <c r="O106" s="0" t="n">
+        <f aca="false">CORREL(O4:O102,$AZ4:$AZ102)</f>
+        <v>0.912418414912747</v>
+      </c>
+      <c r="P106" s="0" t="n">
+        <f aca="false">CORREL(P4:P102,$AZ4:$AZ102)</f>
+        <v>0.923415040949311</v>
+      </c>
+      <c r="Q106" s="0" t="n">
+        <f aca="false">CORREL(Q4:Q102,$AZ4:$AZ102)</f>
+        <v>0.912898314340704</v>
+      </c>
+      <c r="R106" s="0" t="n">
+        <f aca="false">CORREL(R4:R102,$AZ4:$AZ102)</f>
+        <v>0.908983803888801</v>
+      </c>
+      <c r="S106" s="0" t="n">
+        <f aca="false">CORREL(S4:S102,$AZ4:$AZ102)</f>
+        <v>0.915552423617073</v>
+      </c>
+      <c r="T106" s="0" t="n">
+        <f aca="false">CORREL(T4:T102,$AZ4:$AZ102)</f>
+        <v>0.916223833312452</v>
+      </c>
+      <c r="U106" s="0" t="n">
+        <f aca="false">CORREL(U4:U102,$AZ4:$AZ102)</f>
+        <v>0.922040801449228</v>
+      </c>
+      <c r="V106" s="0" t="n">
+        <f aca="false">CORREL(V4:V102,$AZ4:$AZ102)</f>
+        <v>0.926136087355543</v>
+      </c>
+      <c r="W106" s="0" t="n">
+        <f aca="false">CORREL(W4:W102,$AZ4:$AZ102)</f>
+        <v>0.930301246243069</v>
+      </c>
+      <c r="X106" s="0" t="n">
+        <f aca="false">CORREL(X4:X102,$AZ4:$AZ102)</f>
+        <v>0.932313627915127</v>
+      </c>
+      <c r="Y106" s="0" t="n">
+        <f aca="false">CORREL(Y4:Y102,$AZ4:$AZ102)</f>
+        <v>0.93748347865116</v>
+      </c>
+      <c r="Z106" s="0" t="n">
+        <f aca="false">CORREL(Z4:Z102,$AZ4:$AZ102)</f>
+        <v>0.943853343510059</v>
+      </c>
+      <c r="AA106" s="0" t="n">
+        <f aca="false">CORREL(AA4:AA102,$AZ4:$AZ102)</f>
+        <v>0.946543865866151</v>
+      </c>
+      <c r="AB106" s="0" t="n">
+        <f aca="false">CORREL(AB4:AB102,$AZ4:$AZ102)</f>
+        <v>0.949330628145928</v>
+      </c>
+      <c r="AC106" s="0" t="n">
+        <f aca="false">CORREL(AC4:AC102,$AZ4:$AZ102)</f>
+        <v>0.949450608643849</v>
+      </c>
+      <c r="AD106" s="0" t="n">
+        <f aca="false">CORREL(AD4:AD102,$AZ4:$AZ102)</f>
+        <v>0.95591982487483</v>
+      </c>
+      <c r="AE106" s="0" t="n">
+        <f aca="false">CORREL(AE4:AE102,$AZ4:$AZ102)</f>
+        <v>0.962044291085088</v>
+      </c>
+      <c r="AF106" s="0" t="n">
+        <f aca="false">CORREL(AF4:AF102,$AZ4:$AZ102)</f>
+        <v>0.968407646499506</v>
+      </c>
+      <c r="AG106" s="0" t="n">
+        <f aca="false">CORREL(AG4:AG102,$AZ4:$AZ102)</f>
+        <v>0.971708910663133</v>
+      </c>
+      <c r="AH106" s="0" t="n">
+        <f aca="false">CORREL(AH4:AH102,$AZ4:$AZ102)</f>
+        <v>0.974516169364587</v>
+      </c>
+      <c r="AI106" s="0" t="n">
+        <f aca="false">CORREL(AI4:AI102,$AZ4:$AZ102)</f>
+        <v>0.977313963177358</v>
+      </c>
+      <c r="AJ106" s="0" t="n">
+        <f aca="false">CORREL(AJ4:AJ102,$AZ4:$AZ102)</f>
+        <v>0.975459307503107</v>
+      </c>
+      <c r="AK106" s="0" t="n">
+        <f aca="false">CORREL(AK4:AK102,$AZ4:$AZ102)</f>
+        <v>0.977239572543271</v>
+      </c>
+      <c r="AL106" s="0" t="n">
+        <f aca="false">CORREL(AL4:AL102,$AZ4:$AZ102)</f>
+        <v>0.980889849507345</v>
+      </c>
+      <c r="AM106" s="0" t="n">
+        <f aca="false">CORREL(AM4:AM102,$AZ4:$AZ102)</f>
+        <v>0.98613709946611</v>
+      </c>
+      <c r="AN106" s="0" t="n">
+        <f aca="false">CORREL(AN4:AN102,$AZ4:$AZ102)</f>
+        <v>0.987808289252322</v>
+      </c>
+      <c r="AO106" s="0" t="n">
+        <f aca="false">CORREL(AO4:AO102,$AZ4:$AZ102)</f>
+        <v>0.989909318070036</v>
+      </c>
+      <c r="AP106" s="0" t="n">
+        <f aca="false">CORREL(AP4:AP102,$AZ4:$AZ102)</f>
+        <v>0.991487662647391</v>
+      </c>
+      <c r="AQ106" s="0" t="n">
+        <f aca="false">CORREL(AQ4:AQ102,$AZ4:$AZ102)</f>
+        <v>0.993088405280927</v>
+      </c>
+      <c r="AR106" s="0" t="n">
+        <f aca="false">CORREL(AR4:AR102,$AZ4:$AZ102)</f>
+        <v>0.992684656455962</v>
+      </c>
+      <c r="AS106" s="0" t="n">
+        <f aca="false">CORREL(AS4:AS102,$AZ4:$AZ102)</f>
+        <v>0.995382267948756</v>
+      </c>
+      <c r="AT106" s="0" t="n">
+        <f aca="false">CORREL(AT4:AT102,$AZ4:$AZ102)</f>
+        <v>0.995692404909804</v>
+      </c>
+      <c r="AU106" s="0" t="n">
+        <f aca="false">CORREL(AU4:AU102,$AZ4:$AZ102)</f>
+        <v>0.995731031601226</v>
+      </c>
+      <c r="AV106" s="0" t="n">
+        <f aca="false">CORREL(AV4:AV102,$AZ4:$AZ102)</f>
+        <v>0.997697861688746</v>
+      </c>
+      <c r="AW106" s="0" t="n">
+        <f aca="false">CORREL(AW4:AW102,$AZ4:$AZ102)</f>
+        <v>0.99863288504106</v>
+      </c>
+      <c r="AX106" s="0" t="n">
+        <f aca="false">CORREL(AX4:AX102,$AZ4:$AZ102)</f>
+        <v>0.998692740524861</v>
+      </c>
+      <c r="AY106" s="0" t="n">
+        <f aca="false">CORREL(AY4:AY102,$AZ4:$AZ102)</f>
+        <v>0.999314422151944</v>
+      </c>
+      <c r="AZ106" s="0" t="n">
+        <f aca="false">CORREL(AZ4:AZ102,$AZ4:$AZ102)</f>
+        <v>1</v>
+      </c>
+      <c r="BA106" s="0" t="n">
+        <f aca="false">CORREL(BA4:BA102,$AZ4:$AZ102)</f>
+        <v>-0.229213531203459</v>
+      </c>
+      <c r="BB106" s="0" t="n">
+        <f aca="false">CORREL(BB4:BB102,$AZ4:$AZ102)</f>
+        <v>0.80514282563901</v>
+      </c>
+      <c r="BC106" s="0" t="n">
+        <f aca="false">CORREL(BC4:BC102,$AZ4:$AZ102)</f>
+        <v>0.802220045557698</v>
+      </c>
+      <c r="BD106" s="0" t="n">
+        <f aca="false">CORREL(BD4:BD102,$AZ4:$AZ102)</f>
+        <v>0.813370264539875</v>
+      </c>
+      <c r="BE106" s="0" t="n">
+        <f aca="false">CORREL(BE4:BE102,$AZ4:$AZ102)</f>
+        <v>0.829405834741165</v>
+      </c>
+      <c r="BF106" s="0" t="n">
+        <f aca="false">CORREL(BF4:BF102,$AZ4:$AZ102)</f>
+        <v>0.84141081160019</v>
+      </c>
+      <c r="BG106" s="0" t="n">
+        <f aca="false">CORREL(BG4:BG102,$AZ4:$AZ102)</f>
+        <v>0.851188141050979</v>
+      </c>
+      <c r="BH106" s="0" t="n">
+        <f aca="false">CORREL(BH4:BH102,$AZ4:$AZ102)</f>
+        <v>0.855585348703084</v>
+      </c>
+      <c r="BI106" s="0" t="n">
+        <f aca="false">CORREL(BI4:BI102,$AZ4:$AZ102)</f>
+        <v>0.862255874929356</v>
+      </c>
+      <c r="BJ106" s="0" t="n">
+        <f aca="false">CORREL(BJ4:BJ102,$AZ4:$AZ102)</f>
+        <v>0.866700278538914</v>
+      </c>
+      <c r="BK106" s="0" t="n">
+        <f aca="false">CORREL(BK4:BK102,$AZ4:$AZ102)</f>
+        <v>0.86357982200234</v>
+      </c>
+      <c r="BL106" s="0" t="n">
+        <f aca="false">CORREL(BL4:BL102,$AZ4:$AZ102)</f>
+        <v>0.849224119322471</v>
+      </c>
+      <c r="BM106" s="0" t="n">
+        <f aca="false">CORREL(BM4:BM102,$AZ4:$AZ102)</f>
+        <v>0.819063601824044</v>
+      </c>
+      <c r="BN106" s="0" t="n">
+        <f aca="false">CORREL(BN4:BN102,$AZ4:$AZ102)</f>
+        <v>0.764165408996815</v>
+      </c>
+      <c r="BO106" s="0" t="n">
+        <f aca="false">CORREL(BO4:BO102,$AZ4:$AZ102)</f>
+        <v>0.656210333076534</v>
+      </c>
+      <c r="BP106" s="0" t="n">
+        <f aca="false">CORREL(BP4:BP102,$AZ4:$AZ102)</f>
+        <v>0.651739196321154</v>
+      </c>
+      <c r="BQ106" s="0" t="n">
+        <f aca="false">CORREL(BQ4:BQ102,$AZ4:$AZ102)</f>
+        <v>0.624783168232899</v>
+      </c>
+      <c r="BR106" s="0" t="n">
+        <f aca="false">CORREL(BR4:BR102,$AZ4:$AZ102)</f>
+        <v>0.56456168071298</v>
+      </c>
+      <c r="BS106" s="0" t="n">
+        <f aca="false">CORREL(BS4:BS102,$AZ4:$AZ102)</f>
+        <v>0.53100905512749</v>
+      </c>
+      <c r="BT106" s="0" t="n">
+        <f aca="false">CORREL(BT4:BT102,$AZ4:$AZ102)</f>
+        <v>0.412286333303526</v>
+      </c>
+      <c r="BU106" s="0" t="n">
+        <f aca="false">CORREL(BU4:BU102,$AZ4:$AZ102)</f>
+        <v>0.39687794418944</v>
+      </c>
+      <c r="BV106" s="0" t="n">
+        <f aca="false">CORREL(BV4:BV102,$AZ4:$AZ102)</f>
+        <v>0.308830814375195</v>
+      </c>
+      <c r="BW106" s="0" t="n">
+        <f aca="false">CORREL(BW4:BW102,$AZ4:$AZ102)</f>
+        <v>0.273556306730532</v>
+      </c>
+      <c r="BX106" s="0" t="n">
+        <f aca="false">CORREL(BX4:BX102,$AZ4:$AZ102)</f>
+        <v>0.221745028986444</v>
+      </c>
+      <c r="BY106" s="0" t="n">
+        <f aca="false">CORREL(BY4:BY102,$AZ4:$AZ102)</f>
+        <v>0.145116564015874</v>
+      </c>
+      <c r="BZ106" s="0" t="n">
+        <f aca="false">CORREL(BZ4:BZ102,$AZ4:$AZ102)</f>
+        <v>0.0593855982928093</v>
+      </c>
+      <c r="CA106" s="0" t="n">
+        <f aca="false">CORREL(CA4:CA102,$AZ4:$AZ102)</f>
+        <v>0.000183654254070663</v>
+      </c>
+      <c r="CB106" s="0" t="n">
+        <f aca="false">CORREL(CB4:CB102,$AZ4:$AZ102)</f>
+        <v>-0.0613065672992304</v>
+      </c>
+      <c r="CC106" s="0" t="n">
+        <f aca="false">CORREL(CC4:CC102,$AZ4:$AZ102)</f>
+        <v>-0.133018045498109</v>
+      </c>
+      <c r="CD106" s="0" t="n">
+        <f aca="false">CORREL(CD4:CD102,$AZ4:$AZ102)</f>
+        <v>-0.169867562686392</v>
+      </c>
+      <c r="CE106" s="0" t="n">
+        <f aca="false">CORREL(CE4:CE102,$AZ4:$AZ102)</f>
+        <v>-0.19137245286767</v>
+      </c>
+      <c r="CF106" s="0" t="n">
+        <f aca="false">CORREL(CF4:CF102,$AZ4:$AZ102)</f>
+        <v>-0.240894479190407</v>
+      </c>
+      <c r="CG106" s="0" t="n">
+        <f aca="false">CORREL(CG4:CG102,$AZ4:$AZ102)</f>
+        <v>-0.317875952388748</v>
+      </c>
+      <c r="CH106" s="0" t="n">
+        <f aca="false">CORREL(CH4:CH102,$AZ4:$AZ102)</f>
+        <v>-0.361134000668218</v>
+      </c>
+      <c r="CI106" s="0" t="n">
+        <f aca="false">CORREL(CI4:CI102,$AZ4:$AZ102)</f>
+        <v>-0.392165233176521</v>
+      </c>
+      <c r="CJ106" s="0" t="n">
+        <f aca="false">CORREL(CJ4:CJ102,$AZ4:$AZ102)</f>
+        <v>-0.420871292773728</v>
+      </c>
+      <c r="CK106" s="0" t="n">
+        <f aca="false">CORREL(CK4:CK102,$AZ4:$AZ102)</f>
+        <v>-0.43360606561552</v>
+      </c>
+      <c r="CL106" s="0" t="n">
+        <f aca="false">CORREL(CL4:CL102,$AZ4:$AZ102)</f>
+        <v>-0.424732360265747</v>
+      </c>
+      <c r="CM106" s="0" t="n">
+        <f aca="false">CORREL(CM4:CM102,$AZ4:$AZ102)</f>
+        <v>-0.437120273228809</v>
+      </c>
+      <c r="CN106" s="0" t="n">
+        <f aca="false">CORREL(CN4:CN102,$AZ4:$AZ102)</f>
+        <v>-0.469275602116475</v>
+      </c>
+      <c r="CO106" s="0" t="n">
+        <f aca="false">CORREL(CO4:CO102,$AZ4:$AZ102)</f>
+        <v>-0.464016245914042</v>
+      </c>
+      <c r="CP106" s="0" t="n">
+        <f aca="false">CORREL(CP4:CP102,$AZ4:$AZ102)</f>
+        <v>-0.464247825211956</v>
+      </c>
+      <c r="CQ106" s="0" t="n">
+        <f aca="false">CORREL(CQ4:CQ102,$AZ4:$AZ102)</f>
+        <v>-0.491132122839597</v>
+      </c>
+      <c r="CR106" s="0" t="n">
+        <f aca="false">CORREL(CR4:CR102,$AZ4:$AZ102)</f>
+        <v>-0.497156887558805</v>
+      </c>
+      <c r="CS106" s="0" t="n">
+        <f aca="false">CORREL(CS4:CS102,$AZ4:$AZ102)</f>
+        <v>-0.505720009365175</v>
+      </c>
+      <c r="CT106" s="0" t="n">
+        <f aca="false">CORREL(CT4:CT102,$AZ4:$AZ102)</f>
+        <v>-0.525701991034061</v>
+      </c>
+      <c r="CU106" s="0" t="n">
+        <f aca="false">CORREL(CU4:CU102,$AZ4:$AZ102)</f>
+        <v>-0.527432353454656</v>
+      </c>
+      <c r="CV106" s="0" t="n">
+        <f aca="false">CORREL(CV4:CV102,$AZ4:$AZ102)</f>
+        <v>-0.530926865403083</v>
+      </c>
+      <c r="CW106" s="0" t="n">
+        <f aca="false">CORREL(CW4:CW102,$AZ4:$AZ102)</f>
+        <v>-0.532901887594483</v>
+      </c>
+      <c r="CX106" s="0" t="n">
+        <f aca="false">CORREL(CX4:CX102,$AZ4:$AZ102)</f>
+        <v>-0.535447919161507</v>
+      </c>
+      <c r="CY106" s="0" t="n">
+        <f aca="false">CORREL(CY4:CY102,$AZ4:$AZ102)</f>
+        <v>-0.536944173186084</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <f aca="false">CORREL(B4:B102,$CY4:$CY102)</f>
+        <v>0.0475832780109483</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <f aca="false">CORREL(C4:C102,$CY4:$CY102)</f>
+        <v>-0.41704206448687</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <f aca="false">CORREL(D4:D102,$CY4:$CY102)</f>
+        <v>-0.406238671761753</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <f aca="false">CORREL(E4:E102,$CY4:$CY102)</f>
+        <v>-0.415857271315261</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <f aca="false">CORREL(F4:F102,$CY4:$CY102)</f>
+        <v>-0.440531776598524</v>
+      </c>
+      <c r="G107" s="0" t="n">
+        <f aca="false">CORREL(G4:G102,$CY4:$CY102)</f>
+        <v>-0.461046355513544</v>
+      </c>
+      <c r="H107" s="0" t="n">
+        <f aca="false">CORREL(H4:H102,$CY4:$CY102)</f>
+        <v>-0.477279920313145</v>
+      </c>
+      <c r="I107" s="0" t="n">
+        <f aca="false">CORREL(I4:I102,$CY4:$CY102)</f>
+        <v>-0.48732754570834</v>
+      </c>
+      <c r="J107" s="0" t="n">
+        <f aca="false">CORREL(J4:J102,$CY4:$CY102)</f>
+        <v>-0.497585362346604</v>
+      </c>
+      <c r="K107" s="0" t="n">
+        <f aca="false">CORREL(K4:K102,$CY4:$CY102)</f>
+        <v>-0.506673478504868</v>
+      </c>
+      <c r="L107" s="0" t="n">
+        <f aca="false">CORREL(L4:L102,$CY4:$CY102)</f>
+        <v>-0.515300380988852</v>
+      </c>
+      <c r="M107" s="0" t="n">
+        <f aca="false">CORREL(M4:M102,$CY4:$CY102)</f>
+        <v>-0.523118008346956</v>
+      </c>
+      <c r="N107" s="0" t="n">
+        <f aca="false">CORREL(N4:N102,$CY4:$CY102)</f>
+        <v>-0.530627353484659</v>
+      </c>
+      <c r="O107" s="0" t="n">
+        <f aca="false">CORREL(O4:O102,$CY4:$CY102)</f>
+        <v>-0.53648089467515</v>
+      </c>
+      <c r="P107" s="0" t="n">
+        <f aca="false">CORREL(P4:P102,$CY4:$CY102)</f>
+        <v>-0.543198318825201</v>
+      </c>
+      <c r="Q107" s="0" t="n">
+        <f aca="false">CORREL(Q4:Q102,$CY4:$CY102)</f>
+        <v>-0.547988279432831</v>
+      </c>
+      <c r="R107" s="0" t="n">
+        <f aca="false">CORREL(R4:R102,$CY4:$CY102)</f>
+        <v>-0.550653949080961</v>
+      </c>
+      <c r="S107" s="0" t="n">
+        <f aca="false">CORREL(S4:S102,$CY4:$CY102)</f>
+        <v>-0.555260706806816</v>
+      </c>
+      <c r="T107" s="0" t="n">
+        <f aca="false">CORREL(T4:T102,$CY4:$CY102)</f>
+        <v>-0.55662098501949</v>
+      </c>
+      <c r="U107" s="0" t="n">
+        <f aca="false">CORREL(U4:U102,$CY4:$CY102)</f>
+        <v>-0.560253549710787</v>
+      </c>
+      <c r="V107" s="0" t="n">
+        <f aca="false">CORREL(V4:V102,$CY4:$CY102)</f>
+        <v>-0.561742035744227</v>
+      </c>
+      <c r="W107" s="0" t="n">
+        <f aca="false">CORREL(W4:W102,$CY4:$CY102)</f>
+        <v>-0.559578627889997</v>
+      </c>
+      <c r="X107" s="0" t="n">
+        <f aca="false">CORREL(X4:X102,$CY4:$CY102)</f>
+        <v>-0.558412431743802</v>
+      </c>
+      <c r="Y107" s="0" t="n">
+        <f aca="false">CORREL(Y4:Y102,$CY4:$CY102)</f>
+        <v>-0.555946574168229</v>
+      </c>
+      <c r="Z107" s="0" t="n">
+        <f aca="false">CORREL(Z4:Z102,$CY4:$CY102)</f>
+        <v>-0.555913822284466</v>
+      </c>
+      <c r="AA107" s="0" t="n">
+        <f aca="false">CORREL(AA4:AA102,$CY4:$CY102)</f>
+        <v>-0.553996413588177</v>
+      </c>
+      <c r="AB107" s="0" t="n">
+        <f aca="false">CORREL(AB4:AB102,$CY4:$CY102)</f>
+        <v>-0.554616999872939</v>
+      </c>
+      <c r="AC107" s="0" t="n">
+        <f aca="false">CORREL(AC4:AC102,$CY4:$CY102)</f>
+        <v>-0.551684955548093</v>
+      </c>
+      <c r="AD107" s="0" t="n">
+        <f aca="false">CORREL(AD4:AD102,$CY4:$CY102)</f>
+        <v>-0.54705052705929</v>
+      </c>
+      <c r="AE107" s="0" t="n">
+        <f aca="false">CORREL(AE4:AE102,$CY4:$CY102)</f>
+        <v>-0.548020393965442</v>
+      </c>
+      <c r="AF107" s="0" t="n">
+        <f aca="false">CORREL(AF4:AF102,$CY4:$CY102)</f>
+        <v>-0.551806676190149</v>
+      </c>
+      <c r="AG107" s="0" t="n">
+        <f aca="false">CORREL(AG4:AG102,$CY4:$CY102)</f>
+        <v>-0.553096067916515</v>
+      </c>
+      <c r="AH107" s="0" t="n">
+        <f aca="false">CORREL(AH4:AH102,$CY4:$CY102)</f>
+        <v>-0.551106374081489</v>
+      </c>
+      <c r="AI107" s="0" t="n">
+        <f aca="false">CORREL(AI4:AI102,$CY4:$CY102)</f>
+        <v>-0.553782655537892</v>
+      </c>
+      <c r="AJ107" s="0" t="n">
+        <f aca="false">CORREL(AJ4:AJ102,$CY4:$CY102)</f>
+        <v>-0.549841062394162</v>
+      </c>
+      <c r="AK107" s="0" t="n">
+        <f aca="false">CORREL(AK4:AK102,$CY4:$CY102)</f>
+        <v>-0.55137105924221</v>
+      </c>
+      <c r="AL107" s="0" t="n">
+        <f aca="false">CORREL(AL4:AL102,$CY4:$CY102)</f>
+        <v>-0.554820411547878</v>
+      </c>
+      <c r="AM107" s="0" t="n">
+        <f aca="false">CORREL(AM4:AM102,$CY4:$CY102)</f>
+        <v>-0.556950219036183</v>
+      </c>
+      <c r="AN107" s="0" t="n">
+        <f aca="false">CORREL(AN4:AN102,$CY4:$CY102)</f>
+        <v>-0.556918549470756</v>
+      </c>
+      <c r="AO107" s="0" t="n">
+        <f aca="false">CORREL(AO4:AO102,$CY4:$CY102)</f>
+        <v>-0.558642524521228</v>
+      </c>
+      <c r="AP107" s="0" t="n">
+        <f aca="false">CORREL(AP4:AP102,$CY4:$CY102)</f>
+        <v>-0.551984151799189</v>
+      </c>
+      <c r="AQ107" s="0" t="n">
+        <f aca="false">CORREL(AQ4:AQ102,$CY4:$CY102)</f>
+        <v>-0.543550143325468</v>
+      </c>
+      <c r="AR107" s="0" t="n">
+        <f aca="false">CORREL(AR4:AR102,$CY4:$CY102)</f>
+        <v>-0.53619305244642</v>
+      </c>
+      <c r="AS107" s="0" t="n">
+        <f aca="false">CORREL(AS4:AS102,$CY4:$CY102)</f>
+        <v>-0.54145175648661</v>
+      </c>
+      <c r="AT107" s="0" t="n">
+        <f aca="false">CORREL(AT4:AT102,$CY4:$CY102)</f>
+        <v>-0.544805098012692</v>
+      </c>
+      <c r="AU107" s="0" t="n">
+        <f aca="false">CORREL(AU4:AU102,$CY4:$CY102)</f>
+        <v>-0.552694675048098</v>
+      </c>
+      <c r="AV107" s="0" t="n">
+        <f aca="false">CORREL(AV4:AV102,$CY4:$CY102)</f>
+        <v>-0.558469910459338</v>
+      </c>
+      <c r="AW107" s="0" t="n">
+        <f aca="false">CORREL(AW4:AW102,$CY4:$CY102)</f>
+        <v>-0.548903360315757</v>
+      </c>
+      <c r="AX107" s="0" t="n">
+        <f aca="false">CORREL(AX4:AX102,$CY4:$CY102)</f>
+        <v>-0.531782258521124</v>
+      </c>
+      <c r="AY107" s="0" t="n">
+        <f aca="false">CORREL(AY4:AY102,$CY4:$CY102)</f>
+        <v>-0.537520466773574</v>
+      </c>
+      <c r="AZ107" s="0" t="n">
+        <f aca="false">CORREL(AZ4:AZ102,$CY4:$CY102)</f>
+        <v>-0.536944173186084</v>
+      </c>
+      <c r="BA107" s="0" t="n">
+        <f aca="false">CORREL(BA4:BA102,$CY4:$CY102)</f>
+        <v>0.0487411088500321</v>
+      </c>
+      <c r="BB107" s="0" t="n">
+        <f aca="false">CORREL(BB4:BB102,$CY4:$CY102)</f>
+        <v>-0.362661948490413</v>
+      </c>
+      <c r="BC107" s="0" t="n">
+        <f aca="false">CORREL(BC4:BC102,$CY4:$CY102)</f>
+        <v>-0.336703332682763</v>
+      </c>
+      <c r="BD107" s="0" t="n">
+        <f aca="false">CORREL(BD4:BD102,$CY4:$CY102)</f>
+        <v>-0.328914076038715</v>
+      </c>
+      <c r="BE107" s="0" t="n">
+        <f aca="false">CORREL(BE4:BE102,$CY4:$CY102)</f>
+        <v>-0.342511120037622</v>
+      </c>
+      <c r="BF107" s="0" t="n">
+        <f aca="false">CORREL(BF4:BF102,$CY4:$CY102)</f>
+        <v>-0.348225167810312</v>
+      </c>
+      <c r="BG107" s="0" t="n">
+        <f aca="false">CORREL(BG4:BG102,$CY4:$CY102)</f>
+        <v>-0.348274539968563</v>
+      </c>
+      <c r="BH107" s="0" t="n">
+        <f aca="false">CORREL(BH4:BH102,$CY4:$CY102)</f>
+        <v>-0.340779902013266</v>
+      </c>
+      <c r="BI107" s="0" t="n">
+        <f aca="false">CORREL(BI4:BI102,$CY4:$CY102)</f>
+        <v>-0.335129315496345</v>
+      </c>
+      <c r="BJ107" s="0" t="n">
+        <f aca="false">CORREL(BJ4:BJ102,$CY4:$CY102)</f>
+        <v>-0.323067272322146</v>
+      </c>
+      <c r="BK107" s="0" t="n">
+        <f aca="false">CORREL(BK4:BK102,$CY4:$CY102)</f>
+        <v>-0.301497735151381</v>
+      </c>
+      <c r="BL107" s="0" t="n">
+        <f aca="false">CORREL(BL4:BL102,$CY4:$CY102)</f>
+        <v>-0.269231068863772</v>
+      </c>
+      <c r="BM107" s="0" t="n">
+        <f aca="false">CORREL(BM4:BM102,$CY4:$CY102)</f>
+        <v>-0.225758918302248</v>
+      </c>
+      <c r="BN107" s="0" t="n">
+        <f aca="false">CORREL(BN4:BN102,$CY4:$CY102)</f>
+        <v>-0.168308185025999</v>
+      </c>
+      <c r="BO107" s="0" t="n">
+        <f aca="false">CORREL(BO4:BO102,$CY4:$CY102)</f>
+        <v>-0.0890015325398646</v>
+      </c>
+      <c r="BP107" s="0" t="n">
+        <f aca="false">CORREL(BP4:BP102,$CY4:$CY102)</f>
+        <v>-0.0632393151547126</v>
+      </c>
+      <c r="BQ107" s="0" t="n">
+        <f aca="false">CORREL(BQ4:BQ102,$CY4:$CY102)</f>
+        <v>-0.0241999694654896</v>
+      </c>
+      <c r="BR107" s="0" t="n">
+        <f aca="false">CORREL(BR4:BR102,$CY4:$CY102)</f>
+        <v>0.0308696131444579</v>
+      </c>
+      <c r="BS107" s="0" t="n">
+        <f aca="false">CORREL(BS4:BS102,$CY4:$CY102)</f>
+        <v>0.0792244187703312</v>
+      </c>
+      <c r="BT107" s="0" t="n">
+        <f aca="false">CORREL(BT4:BT102,$CY4:$CY102)</f>
+        <v>0.157317166420492</v>
+      </c>
+      <c r="BU107" s="0" t="n">
+        <f aca="false">CORREL(BU4:BU102,$CY4:$CY102)</f>
+        <v>0.202041266945999</v>
+      </c>
+      <c r="BV107" s="0" t="n">
+        <f aca="false">CORREL(BV4:BV102,$CY4:$CY102)</f>
+        <v>0.276288187901393</v>
+      </c>
+      <c r="BW107" s="0" t="n">
+        <f aca="false">CORREL(BW4:BW102,$CY4:$CY102)</f>
+        <v>0.332545668746539</v>
+      </c>
+      <c r="BX107" s="0" t="n">
+        <f aca="false">CORREL(BX4:BX102,$CY4:$CY102)</f>
+        <v>0.384392851493785</v>
+      </c>
+      <c r="BY107" s="0" t="n">
+        <f aca="false">CORREL(BY4:BY102,$CY4:$CY102)</f>
+        <v>0.437468348152137</v>
+      </c>
+      <c r="BZ107" s="0" t="n">
+        <f aca="false">CORREL(BZ4:BZ102,$CY4:$CY102)</f>
+        <v>0.504631513628478</v>
+      </c>
+      <c r="CA107" s="0" t="n">
+        <f aca="false">CORREL(CA4:CA102,$CY4:$CY102)</f>
+        <v>0.561825752330906</v>
+      </c>
+      <c r="CB107" s="0" t="n">
+        <f aca="false">CORREL(CB4:CB102,$CY4:$CY102)</f>
+        <v>0.621152213490523</v>
+      </c>
+      <c r="CC107" s="0" t="n">
+        <f aca="false">CORREL(CC4:CC102,$CY4:$CY102)</f>
+        <v>0.673706340957417</v>
+      </c>
+      <c r="CD107" s="0" t="n">
+        <f aca="false">CORREL(CD4:CD102,$CY4:$CY102)</f>
+        <v>0.721876641584547</v>
+      </c>
+      <c r="CE107" s="0" t="n">
+        <f aca="false">CORREL(CE4:CE102,$CY4:$CY102)</f>
+        <v>0.763669399216473</v>
+      </c>
+      <c r="CF107" s="0" t="n">
+        <f aca="false">CORREL(CF4:CF102,$CY4:$CY102)</f>
+        <v>0.795143838842246</v>
+      </c>
+      <c r="CG107" s="0" t="n">
+        <f aca="false">CORREL(CG4:CG102,$CY4:$CY102)</f>
+        <v>0.816706134008494</v>
+      </c>
+      <c r="CH107" s="0" t="n">
+        <f aca="false">CORREL(CH4:CH102,$CY4:$CY102)</f>
+        <v>0.82411235583664</v>
+      </c>
+      <c r="CI107" s="0" t="n">
+        <f aca="false">CORREL(CI4:CI102,$CY4:$CY102)</f>
+        <v>0.826611450489542</v>
+      </c>
+      <c r="CJ107" s="0" t="n">
+        <f aca="false">CORREL(CJ4:CJ102,$CY4:$CY102)</f>
+        <v>0.848122123084888</v>
+      </c>
+      <c r="CK107" s="0" t="n">
+        <f aca="false">CORREL(CK4:CK102,$CY4:$CY102)</f>
+        <v>0.878623349318221</v>
+      </c>
+      <c r="CL107" s="0" t="n">
+        <f aca="false">CORREL(CL4:CL102,$CY4:$CY102)</f>
+        <v>0.907806995936771</v>
+      </c>
+      <c r="CM107" s="0" t="n">
+        <f aca="false">CORREL(CM4:CM102,$CY4:$CY102)</f>
+        <v>0.920843249388175</v>
+      </c>
+      <c r="CN107" s="0" t="n">
+        <f aca="false">CORREL(CN4:CN102,$CY4:$CY102)</f>
+        <v>0.936741538536239</v>
+      </c>
+      <c r="CO107" s="0" t="n">
+        <f aca="false">CORREL(CO4:CO102,$CY4:$CY102)</f>
+        <v>0.952705896270968</v>
+      </c>
+      <c r="CP107" s="0" t="n">
+        <f aca="false">CORREL(CP4:CP102,$CY4:$CY102)</f>
+        <v>0.961481345478428</v>
+      </c>
+      <c r="CQ107" s="0" t="n">
+        <f aca="false">CORREL(CQ4:CQ102,$CY4:$CY102)</f>
+        <v>0.962482603250768</v>
+      </c>
+      <c r="CR107" s="0" t="n">
+        <f aca="false">CORREL(CR4:CR102,$CY4:$CY102)</f>
+        <v>0.971010405691419</v>
+      </c>
+      <c r="CS107" s="0" t="n">
+        <f aca="false">CORREL(CS4:CS102,$CY4:$CY102)</f>
+        <v>0.981833347480896</v>
+      </c>
+      <c r="CT107" s="0" t="n">
+        <f aca="false">CORREL(CT4:CT102,$CY4:$CY102)</f>
+        <v>0.982050260275274</v>
+      </c>
+      <c r="CU107" s="0" t="n">
+        <f aca="false">CORREL(CU4:CU102,$CY4:$CY102)</f>
+        <v>0.989016000528553</v>
+      </c>
+      <c r="CV107" s="0" t="n">
+        <f aca="false">CORREL(CV4:CV102,$CY4:$CY102)</f>
+        <v>0.995020111196712</v>
+      </c>
+      <c r="CW107" s="0" t="n">
+        <f aca="false">CORREL(CW4:CW102,$CY4:$CY102)</f>
+        <v>0.993802635843499</v>
+      </c>
+      <c r="CX107" s="0" t="n">
+        <f aca="false">CORREL(CX4:CX102,$CY4:$CY102)</f>
+        <v>0.998099930693921</v>
+      </c>
+      <c r="CY107" s="0" t="n">
+        <f aca="false">CORREL(CY4:CY102,$CY4:$CY102)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <f aca="false">CORREL(B4:B102, BA4:BA102)</f>
+        <v>0.999893336769088</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <f aca="false">CORREL(C4:C102, BB4:BB102)</f>
+        <v>0.979565641530459</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <f aca="false">CORREL(D4:D102, BC4:BC102)</f>
+        <v>0.976098632150636</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <f aca="false">CORREL(E4:E102, BD4:BD102)</f>
+        <v>0.968424960717981</v>
+      </c>
+      <c r="F109" s="0" t="n">
+        <f aca="false">CORREL(F4:F102, BE4:BE102)</f>
+        <v>0.96275567965491</v>
+      </c>
+      <c r="G109" s="0" t="n">
+        <f aca="false">CORREL(G4:G102, BF4:BF102)</f>
+        <v>0.957312033534776</v>
+      </c>
+      <c r="H109" s="0" t="n">
+        <f aca="false">CORREL(H4:H102, BG4:BG102)</f>
+        <v>0.950190043443918</v>
+      </c>
+      <c r="I109" s="0" t="n">
+        <f aca="false">CORREL(I4:I102, BH4:BH102)</f>
+        <v>0.941834383269147</v>
+      </c>
+      <c r="J109" s="0" t="n">
+        <f aca="false">CORREL(J4:J102, BI4:BI102)</f>
+        <v>0.930424425268262</v>
+      </c>
+      <c r="K109" s="0" t="n">
+        <f aca="false">CORREL(K4:K102, BJ4:BJ102)</f>
+        <v>0.913029234439695</v>
+      </c>
+      <c r="L109" s="0" t="n">
+        <f aca="false">CORREL(L4:L102, BK4:BK102)</f>
+        <v>0.880865716099726</v>
+      </c>
+      <c r="M109" s="0" t="n">
+        <f aca="false">CORREL(M4:M102, BL4:BL102)</f>
+        <v>0.825304380940406</v>
+      </c>
+      <c r="N109" s="0" t="n">
+        <f aca="false">CORREL(N4:N102, BM4:BM102)</f>
+        <v>0.747197922340749</v>
+      </c>
+      <c r="O109" s="0" t="n">
+        <f aca="false">CORREL(O4:O102, BN4:BN102)</f>
+        <v>0.656180801239611</v>
+      </c>
+      <c r="P109" s="0" t="n">
+        <f aca="false">CORREL(P4:P102, BO4:BO102)</f>
+        <v>0.525956835211211</v>
+      </c>
+      <c r="Q109" s="0" t="n">
+        <f aca="false">CORREL(Q4:Q102, BP4:BP102)</f>
+        <v>0.475596078433006</v>
+      </c>
+      <c r="R109" s="0" t="n">
+        <f aca="false">CORREL(R4:R102, BQ4:BQ102)</f>
+        <v>0.425661465599727</v>
+      </c>
+      <c r="S109" s="0" t="n">
+        <f aca="false">CORREL(S4:S102, BR4:BR102)</f>
+        <v>0.364466271916278</v>
+      </c>
+      <c r="T109" s="0" t="n">
+        <f aca="false">CORREL(T4:T102, BS4:BS102)</f>
+        <v>0.325790196544273</v>
+      </c>
+      <c r="U109" s="0" t="n">
+        <f aca="false">CORREL(U4:U102, BT4:BT102)</f>
+        <v>0.18681282090316</v>
+      </c>
+      <c r="V109" s="0" t="n">
+        <f aca="false">CORREL(V4:V102, BU4:BU102)</f>
+        <v>0.180100993110383</v>
+      </c>
+      <c r="W109" s="0" t="n">
+        <f aca="false">CORREL(W4:W102, BV4:BV102)</f>
+        <v>0.087093061936429</v>
+      </c>
+      <c r="X109" s="0" t="n">
+        <f aca="false">CORREL(X4:X102, BW4:BW102)</f>
+        <v>0.0635277250524798</v>
+      </c>
+      <c r="Y109" s="0" t="n">
+        <f aca="false">CORREL(Y4:Y102, BX4:BX102)</f>
+        <v>0.0250172157311133</v>
+      </c>
+      <c r="Z109" s="0" t="n">
+        <f aca="false">CORREL(Z4:Z102, BY4:BY102)</f>
+        <v>-0.0320858163264702</v>
+      </c>
+      <c r="AA109" s="0" t="n">
+        <f aca="false">CORREL(AA4:AA102, BZ4:BZ102)</f>
+        <v>-0.100747008693178</v>
+      </c>
+      <c r="AB109" s="0" t="n">
+        <f aca="false">CORREL(AB4:AB102, CA4:CA102)</f>
+        <v>-0.135591475078363</v>
+      </c>
+      <c r="AC109" s="0" t="n">
+        <f aca="false">CORREL(AC4:AC102, CB4:CB102)</f>
+        <v>-0.178785883758916</v>
+      </c>
+      <c r="AD109" s="0" t="n">
+        <f aca="false">CORREL(AD4:AD102, CC4:CC102)</f>
+        <v>-0.241606923573501</v>
+      </c>
+      <c r="AE109" s="0" t="n">
+        <f aca="false">CORREL(AE4:AE102, CD4:CD102)</f>
+        <v>-0.272963732366239</v>
+      </c>
+      <c r="AF109" s="0" t="n">
+        <f aca="false">CORREL(AF4:AF102, CE4:CE102)</f>
+        <v>-0.296663017900597</v>
+      </c>
+      <c r="AG109" s="0" t="n">
+        <f aca="false">CORREL(AG4:AG102, CF4:CF102)</f>
+        <v>-0.332437933199911</v>
+      </c>
+      <c r="AH109" s="0" t="n">
+        <f aca="false">CORREL(AH4:AH102, CG4:CG102)</f>
+        <v>-0.393692228249123</v>
+      </c>
+      <c r="AI109" s="0" t="n">
+        <f aca="false">CORREL(AI4:AI102, CH4:CH102)</f>
+        <v>-0.421543995899352</v>
+      </c>
+      <c r="AJ109" s="0" t="n">
+        <f aca="false">CORREL(AJ4:AJ102, CI4:CI102)</f>
+        <v>-0.417499433829198</v>
+      </c>
+      <c r="AK109" s="0" t="n">
+        <f aca="false">CORREL(AK4:AK102, CJ4:CJ102)</f>
+        <v>-0.443805761716125</v>
+      </c>
+      <c r="AL109" s="0" t="n">
+        <f aca="false">CORREL(AL4:AL102, CK4:CK102)</f>
+        <v>-0.459231636989867</v>
+      </c>
+      <c r="AM109" s="0" t="n">
+        <f aca="false">CORREL(AM4:AM102, CL4:CL102)</f>
+        <v>-0.461288669936574</v>
+      </c>
+      <c r="AN109" s="0" t="n">
+        <f aca="false">CORREL(AN4:AN102, CM4:CM102)</f>
+        <v>-0.468019324118815</v>
+      </c>
+      <c r="AO109" s="0" t="n">
+        <f aca="false">CORREL(AO4:AO102, CN4:CN102)</f>
+        <v>-0.502354965150293</v>
+      </c>
+      <c r="AP109" s="0" t="n">
+        <f aca="false">CORREL(AP4:AP102, CO4:CO102)</f>
+        <v>-0.487374778560231</v>
+      </c>
+      <c r="AQ109" s="0" t="n">
+        <f aca="false">CORREL(AQ4:AQ102, CP4:CP102)</f>
+        <v>-0.474437541658581</v>
+      </c>
+      <c r="AR109" s="0" t="n">
+        <f aca="false">CORREL(AR4:AR102, CQ4:CQ102)</f>
+        <v>-0.486082252198933</v>
+      </c>
+      <c r="AS109" s="0" t="n">
+        <f aca="false">CORREL(AS4:AS102, CR4:CR102)</f>
+        <v>-0.50147428495481</v>
+      </c>
+      <c r="AT109" s="0" t="n">
+        <f aca="false">CORREL(AT4:AT102, CS4:CS102)</f>
+        <v>-0.511580833242484</v>
+      </c>
+      <c r="AU109" s="0" t="n">
+        <f aca="false">CORREL(AU4:AU102, CT4:CT102)</f>
+        <v>-0.534427526478777</v>
+      </c>
+      <c r="AV109" s="0" t="n">
+        <f aca="false">CORREL(AV4:AV102, CU4:CU102)</f>
+        <v>-0.546106238658912</v>
+      </c>
+      <c r="AW109" s="0" t="n">
+        <f aca="false">CORREL(AW4:AW102, CV4:CV102)</f>
+        <v>-0.54138985923452</v>
+      </c>
+      <c r="AX109" s="0" t="n">
+        <f aca="false">CORREL(AX4:AX102, CW4:CW102)</f>
+        <v>-0.524663574503246</v>
+      </c>
+      <c r="AY109" s="0" t="n">
+        <f aca="false">CORREL(AY4:AY102, CX4:CX102)</f>
+        <v>-0.534241883921962</v>
+      </c>
+      <c r="AZ109" s="0" t="n">
+        <f aca="false">CORREL(AZ4:AZ102, CY4:CY102)</f>
+        <v>-0.536944173186084</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>